<commit_message>
changes at 12/0/2021 (subclassing engine)
</commit_message>
<xml_diff>
--- a/BotHallWeb/Bot Hall classes.xlsx
+++ b/BotHallWeb/Bot Hall classes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="96">
   <si>
     <t xml:space="preserve">BotHallAPI</t>
   </si>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">disconnects from a bothall session and client, but keeps the socket running</t>
   </si>
   <si>
-    <t xml:space="preserve">BHClientAgent</t>
+    <t xml:space="preserve">BHClientRegistration</t>
   </si>
   <si>
     <r>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t xml:space="preserve">the message queue ID for getting messages from the bothall session; a reference to BHMessageList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userKey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user that created the client</t>
   </si>
   <si>
     <t xml:space="preserve">BHSession</t>
@@ -568,13 +574,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:D94"/>
+  <dimension ref="B3:D95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
@@ -775,25 +781,25 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
-        <v>34</v>
+      <c r="B33" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>46</v>
@@ -816,39 +822,39 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="C37" s="0" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D38" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D40" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D42" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="0" t="s">
+      <c r="B44" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D44" s="0" t="s">
@@ -856,61 +862,58 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D46" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D48" s="0" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>67</v>
+      </c>
       <c r="D50" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="D53" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="0" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>74</v>
@@ -921,108 +924,119 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="D58" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>79</v>
+        <v>65</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="0" t="s">
-        <v>84</v>
+      <c r="B82" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
         <v>87</v>
       </c>
     </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D85" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="0" t="s">
-        <v>88</v>
+      <c r="B87" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D88" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D89" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D90" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="0" t="s">
-        <v>93</v>
+      <c r="B94" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D95" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>